<commit_message>
Predicciones, simulaciones y cumplimiento 2.0.1
</commit_message>
<xml_diff>
--- a/Proyecto1_Limpieza/resultados_analisis_emisiones.xlsx
+++ b/Proyecto1_Limpieza/resultados_analisis_emisiones.xlsx
@@ -8,28 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/506a708389be33d1/Escritorio/portafolio_chilexpress/Proyecto1_Limpieza/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_101CEC462707C0832B7C60985FC65657A2F170D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{457A145C-12ED-4800-A182-6E037261787C}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_101CEC462707C0832B7C60985FC65657A2F170D4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B084694B-DE2D-4557-A910-708650216A67}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Predicciones_2023" sheetId="1" r:id="rId1"/>
     <sheet name="Simulaciones_SBTi" sheetId="2" r:id="rId2"/>
     <sheet name="Evaluacion_SBTi" sheetId="3" r:id="rId3"/>
+    <sheet name="consideraciones" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Subcategoría</t>
   </si>
   <si>
-    <t>Emisiones 2021 (tCO₂e)</t>
-  </si>
-  <si>
     <t>Emisiones 2022 Real (tCO₂e)</t>
   </si>
   <si>
@@ -94,6 +92,171 @@
   </si>
   <si>
     <t>Cumplimiento Global Metas Evaluadas</t>
+  </si>
+  <si>
+    <t>Emisiones 2021 (kCO₂e)</t>
+  </si>
+  <si>
+    <t>"Este modelo es una primera aproximación cuantitativa basada en datos operativos preliminares. Está alineado con los compromisos SBTi de Chilexpress y será refinado con los factores de emisión específicos del sector logístico, en coordinación con el equipo de sostenibilidad corporativa."</t>
+  </si>
+  <si>
+    <t>Categoría</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Discrepancias en el análisis inicial</t>
+  </si>
+  <si>
+    <t>Contexto faltante</t>
+  </si>
+  <si>
+    <t>No se mencionó que Chilexpress ya electrificó el 100% de su flota, lo que explica la baja en "Combustión - fuentes fijas".</t>
+  </si>
+  <si>
+    <t>Unidades malinterpretadas</t>
+  </si>
+  <si>
+    <t>Los datos de "Total encomiendas" (32,943 tCO₂e) parecen altos para una flota electrificada. Es posible que estén en ktCO₂e (kilotoneladas); si es así, los números sí cuadrarían.</t>
+  </si>
+  <si>
+    <t>Falta de vinculación a acciones reales</t>
+  </si>
+  <si>
+    <t>No se vincularon las reducciones a proyectos específicos (ej: electrificación, energía renovable on-site), lo que generó dudas sobre la metodología.</t>
+  </si>
+  <si>
+    <t>Fortalezas del trabajo actual</t>
+  </si>
+  <si>
+    <t>Reducción del 37.6% en emisiones</t>
+  </si>
+  <si>
+    <t>Es coherente con una electrificación agresiva de la flota y el uso de energía renovable.</t>
+  </si>
+  <si>
+    <t>Estructura del script</t>
+  </si>
+  <si>
+    <t>Es replicable y automatizable, ideal para reportes anuales.</t>
+  </si>
+  <si>
+    <t>Cobertura Alcance 3 &gt;90%</t>
+  </si>
+  <si>
+    <t>Demuestra transparencia en la cadena de valor, clave para SBTi.</t>
+  </si>
+  <si>
+    <t>Lista de ajustes para validar con SBTi y GHG Protocol</t>
+  </si>
+  <si>
+    <t>Corrección de datos y unidades</t>
+  </si>
+  <si>
+    <t>Unidades de emisión</t>
+  </si>
+  <si>
+    <t>Se debe verificar si "Total encomiendas" está en tCO₂e o ktCO₂e (19,105 tCO₂e = ~19 ktCO₂e).</t>
+  </si>
+  <si>
+    <t>Desglose Alcance 3</t>
+  </si>
+  <si>
+    <t>Se debe dividir "Total encomiendas" en categorías SBTi:</t>
+  </si>
+  <si>
+    <t>- Transporte terrestre (flota propia vs terceros)</t>
+  </si>
+  <si>
+    <t>- Embalajes (cartón, plástico)</t>
+  </si>
+  <si>
+    <t>- Última milla (vehículos menores)</t>
+  </si>
+  <si>
+    <t>Electrificación flota</t>
+  </si>
+  <si>
+    <t>Se deben incluir datos reales:</t>
+  </si>
+  <si>
+    <t>- N° vehículos eléctricos, consumo kWh/km, fuentes de carga</t>
+  </si>
+  <si>
+    <t>Validación con herramientas oficiales</t>
+  </si>
+  <si>
+    <t>SBTi Target Validation Tool</t>
+  </si>
+  <si>
+    <t>Verifica la coherencia de metas con el sector logístico.</t>
+  </si>
+  <si>
+    <t>GHG Protocol Mobile/Fleet Calculator</t>
+  </si>
+  <si>
+    <t>Calcula emisiones de flota electrificada con datos reales (kWh, km, carga).</t>
+  </si>
+  <si>
+    <t>SBTi FLAG Guide (para embalajes)</t>
+  </si>
+  <si>
+    <t>Asegura que las emisiones de materiales cumplan con criterios de bioeconomía.</t>
+  </si>
+  <si>
+    <t>Cómo contrastar los datos actuales con SBTi</t>
+  </si>
+  <si>
+    <t>Plantilla de reporte SBTi</t>
+  </si>
+  <si>
+    <t>Se debe descargar y completar con los siguientes campos:</t>
+  </si>
+  <si>
+    <t>- Emisiones separadas por Alcance 1 (flota), Alcance 2 (electricidad), Alcance 3 (embalajes, transporte terceros).</t>
+  </si>
+  <si>
+    <t>- Meta de reducción a 2030 vinculada a KPIs operativos (% flota eléctrica, % energía renovable contratada).</t>
+  </si>
+  <si>
+    <t>Simulador de escenarios SBTi</t>
+  </si>
+  <si>
+    <t>Permite probar predicciones para 2023 ingresando datos de 2021-2022 y verificando si la proyección 2023 cumple la trayectoria 1.5°C.</t>
+  </si>
+  <si>
+    <t>Validación de residuos sanitarios</t>
+  </si>
+  <si>
+    <t>Si Chilexpress tiene "0 residuos sanitarios", esto debe reflejarse como reducción en la categoría "Waste generated in operations" (GHG Protocol Category 5).</t>
+  </si>
+  <si>
+    <t>Elementos clave para no descartar el trabajo</t>
+  </si>
+  <si>
+    <t>Anexo 1</t>
+  </si>
+  <si>
+    <t>Certificado SBTi de Chilexpress (demuestra que las metas ya están validadas).</t>
+  </si>
+  <si>
+    <t>Anexo 2</t>
+  </si>
+  <si>
+    <t>Detalle técnico de la electrificación (n° vehículos, autonomía, proveedor de energía).</t>
+  </si>
+  <si>
+    <t>Anexo 3</t>
+  </si>
+  <si>
+    <t>Política de residuos (métodos de reciclaje, % desviación de vertederos).</t>
+  </si>
+  <si>
+    <t>Anexo 4</t>
+  </si>
+  <si>
+    <t>Cálculos de Alcance 3 usando factores del IPCC para transporte de carga.</t>
   </si>
 </sst>
 </file>
@@ -102,10 +265,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +289,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -163,7 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -171,10 +354,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -183,18 +366,56 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -205,6 +426,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31676F8C-9DE1-417D-B480-390F5CCC72D5}" name="Tabla1" displayName="Tabla1" ref="A1:B33" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:B33" xr:uid="{31676F8C-9DE1-417D-B480-390F5CCC72D5}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C13C944B-8520-432F-9E17-D4B952E9C0A8}" name="Categoría" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{60C65EFF-0D42-4618-B127-F42207A3C23A}" name="Observaciones" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,23 +735,23 @@
     <col min="1" max="16384" width="26.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>4.0000000000000001E-3</v>
@@ -531,9 +763,9 @@
         <v>9.7021979602448044E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>1.591</v>
@@ -545,9 +777,9 @@
         <v>0.67550558544319339</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="4">
         <v>0.30299999999999999</v>
@@ -559,9 +791,9 @@
         <v>0.23363325639487889</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4">
         <v>32943.152000000002</v>
@@ -573,7 +805,36 @@
         <v>10526.69201304355</v>
       </c>
     </row>
+    <row r="10" spans="1:7" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F10:G15"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -583,7 +844,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="28.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,15 +854,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
         <v>1.36</v>
@@ -609,7 +870,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3">
         <v>0.28999999999999998</v>
@@ -624,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,15 +896,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="7">
         <v>37.6</v>
@@ -651,7 +912,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7">
         <v>4.2</v>
@@ -659,7 +920,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="7">
         <v>33.4</v>
@@ -667,7 +928,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="7">
         <v>92.9</v>
@@ -675,15 +936,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="6">
         <v>67</v>
@@ -691,29 +952,288 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947ADEF5-2264-4AE9-A3C6-80D0C86EE390}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="67.88671875" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="67.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="10"/>
+    </row>
+    <row r="3" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="10"/>
+    </row>
+    <row r="12" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>